<commit_message>
small changes to the code strucutre
overall the program remains the same, I decided to reword some of the 
documentation and also adjust the excel file for further testing but the 
core functionality has not changed
</commit_message>
<xml_diff>
--- a/data/sample_data.xlsx
+++ b/data/sample_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredmathew/PythonStuff/Email-Sender/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredmathew/PythonStuff/Email-Sender/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE917FE4-FEA1-4945-BFC6-CAAE5F49EB9B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB33F0A2-A2CA-5449-8218-ABCD27300CBD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18160" windowHeight="14500" xr2:uid="{945A9013-496A-45AA-A316-483B626892D7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="133">
   <si>
     <t>Baptized-DOB</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>Sarah19</t>
+  </si>
+  <si>
+    <t>Baptized-Email</t>
+  </si>
+  <si>
+    <t>alfmat@live.unc.edu</t>
   </si>
 </sst>
 </file>
@@ -800,22 +806,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828FD520-B8B1-419E-ADC4-B5D2AE0B127C}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="16" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
+    <col min="16" max="17" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -823,888 +829,910 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1"/>
+      <c r="D2" s="3">
         <v>42957</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>43018</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="1"/>
+      <c r="O2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1"/>
+      <c r="D3" s="3">
         <v>42988</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>43049</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="3">
         <v>43018</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>43095</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="1"/>
+      <c r="O4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1"/>
+      <c r="D5" s="3">
         <v>43049</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>43110</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="1"/>
+      <c r="O5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1"/>
+      <c r="D6" s="3">
         <v>43079</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>43141</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1"/>
+      <c r="D7" s="3">
         <v>43110</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>43169</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="1"/>
+      <c r="O7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1"/>
+      <c r="D8" s="3">
         <v>43141</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>43200</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="1"/>
+      <c r="O8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="3">
         <v>43169</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>43230</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="1"/>
+      <c r="O9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1"/>
+      <c r="D10" s="3">
         <v>43200</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>43261</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="1"/>
+      <c r="O10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1"/>
+      <c r="D11" s="3">
         <v>43230</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>43291</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1" t="s">
+      <c r="N11" s="1"/>
+      <c r="O11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="3">
         <v>43261</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>43322</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1" t="s">
+      <c r="N12" s="1"/>
+      <c r="O12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="1"/>
+      <c r="D13" s="3">
         <v>43291</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>43353</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1" t="s">
+      <c r="N13" s="1"/>
+      <c r="O13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="1"/>
+      <c r="D14" s="3">
         <v>43322</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>43383</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1" t="s">
+      <c r="N14" s="1"/>
+      <c r="O14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="1"/>
+      <c r="D15" s="3">
         <v>43353</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>43414</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1" t="s">
+      <c r="N15" s="1"/>
+      <c r="O15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="1"/>
+      <c r="D16" s="3">
         <v>43383</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>43444</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="1"/>
+      <c r="L16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1" t="s">
+      <c r="N16" s="1"/>
+      <c r="O16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="1"/>
+      <c r="D17" s="3">
         <v>43414</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>43475</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="1"/>
+      <c r="L17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1" t="s">
+      <c r="N17" s="1"/>
+      <c r="O17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="1"/>
+      <c r="D18" s="3">
         <v>43444</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>43506</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1" t="s">
+      <c r="N18" s="1"/>
+      <c r="O18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="P18" s="1"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="1"/>
+      <c r="D19" s="3">
         <v>43475</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <v>43534</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1" t="s">
+      <c r="K19" s="1"/>
+      <c r="L19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1" t="s">
+      <c r="N19" s="1"/>
+      <c r="O19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="1"/>
+      <c r="D20" s="3">
         <v>43506</v>
       </c>
-      <c r="D20" s="3">
-        <v>43565</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="3">
+        <v>43527</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1" t="s">
+      <c r="K20" s="1"/>
+      <c r="L20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1" t="s">
+      <c r="N20" s="1"/>
+      <c r="O20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{26E47728-E3DD-46C8-A5AA-8FA0D936EDC7}"/>
-    <hyperlink ref="G3:G20" r:id="rId2" display="mattsebastian@live.com" xr:uid="{DBBFF14D-4647-4905-9213-A649131D5474}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{26E47728-E3DD-46C8-A5AA-8FA0D936EDC7}"/>
+    <hyperlink ref="H20" r:id="rId2" xr:uid="{6CF34441-E405-3D40-8227-F2C56CD53050}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>